<commit_message>
Data Setup For Product Historical
</commit_message>
<xml_diff>
--- a/ProductHistorical_TestData.xlsx
+++ b/ProductHistorical_TestData.xlsx
@@ -55,11 +55,12 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="2">
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode="GENERAL"/>
     <numFmt numFmtId="165" formatCode="DD/MM/YY"/>
+    <numFmt numFmtId="166" formatCode="DD/MM/YY"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="5">
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
@@ -89,12 +90,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -139,7 +134,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -148,11 +143,15 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -228,10 +227,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:U1"/>
+  <dimension ref="A1:R3"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="I1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="U1" activeCellId="0" sqref="U1"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G6" activeCellId="0" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -248,7 +247,7 @@
     <col collapsed="false" hidden="false" max="1025" min="10" style="0" width="8.36296296296296"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="16.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
         <v>0</v>
       </c>
@@ -276,37 +275,42 @@
       <c r="I1" s="0" t="n">
         <v>10</v>
       </c>
-      <c r="J1" s="0" t="s">
+      <c r="J1" s="0" t="n">
+        <v>20</v>
+      </c>
+      <c r="K1" s="0" t="n">
+        <v>30</v>
+      </c>
+      <c r="R1" s="3"/>
+    </row>
+    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G2" s="4" t="n">
+        <v>43831</v>
+      </c>
+      <c r="H2" s="0" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="0" t="n">
+      <c r="I2" s="0" t="n">
         <v>11</v>
       </c>
-      <c r="L1" s="0" t="s">
+      <c r="J2" s="0" t="n">
+        <v>21</v>
+      </c>
+      <c r="K2" s="0" t="n">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="H3" s="0" t="s">
         <v>10</v>
       </c>
-      <c r="M1" s="0" t="n">
+      <c r="I3" s="0" t="n">
         <v>12</v>
       </c>
-      <c r="O1" s="0" t="n">
-        <v>20</v>
-      </c>
-      <c r="P1" s="0" t="n">
-        <v>21</v>
-      </c>
-      <c r="Q1" s="0" t="n">
+      <c r="J3" s="0" t="n">
         <v>22</v>
       </c>
-      <c r="R1" s="3" t="n">
-        <v>43831</v>
-      </c>
-      <c r="S1" s="0" t="n">
-        <v>30</v>
-      </c>
-      <c r="T1" s="0" t="n">
-        <v>31</v>
-      </c>
-      <c r="U1" s="0" t="n">
+      <c r="K3" s="0" t="n">
         <v>32</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Add Method in BasePage to read the excel data
</commit_message>
<xml_diff>
--- a/ProductHistorical_TestData.xlsx
+++ b/ProductHistorical_TestData.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="11">
   <si>
     <t>admin</t>
   </si>
@@ -227,10 +227,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:R3"/>
+  <dimension ref="A1:R9"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G6" activeCellId="0" sqref="G6"/>
+      <selection pane="topLeft" activeCell="I19" activeCellId="0" sqref="I19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -275,17 +275,14 @@
       <c r="I1" s="0" t="n">
         <v>10</v>
       </c>
-      <c r="J1" s="0" t="n">
-        <v>20</v>
-      </c>
       <c r="K1" s="0" t="n">
         <v>30</v>
       </c>
       <c r="R1" s="3"/>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="G2" s="4" t="n">
-        <v>43831</v>
+      <c r="G2" s="3" t="n">
+        <v>25569</v>
       </c>
       <c r="H2" s="0" t="s">
         <v>9</v>
@@ -293,24 +290,87 @@
       <c r="I2" s="0" t="n">
         <v>11</v>
       </c>
-      <c r="J2" s="0" t="n">
-        <v>21</v>
-      </c>
       <c r="K2" s="0" t="n">
         <v>31</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G3" s="3" t="n">
+        <v>25569</v>
+      </c>
       <c r="H3" s="0" t="s">
         <v>10</v>
       </c>
       <c r="I3" s="0" t="n">
         <v>12</v>
       </c>
-      <c r="J3" s="0" t="n">
+      <c r="K3" s="0" t="n">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G4" s="4" t="n">
+        <v>43276.5385855949</v>
+      </c>
+      <c r="H4" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="I4" s="0" t="n">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G5" s="4" t="n">
+        <v>43276.5385094428</v>
+      </c>
+      <c r="H5" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="I5" s="0" t="n">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G6" s="4" t="n">
+        <v>43276.5385244457</v>
+      </c>
+      <c r="H6" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="I6" s="0" t="n">
         <v>22</v>
       </c>
-      <c r="K3" s="0" t="n">
+    </row>
+    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G7" s="4" t="n">
+        <v>43831</v>
+      </c>
+      <c r="H7" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="I7" s="0" t="n">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G8" s="4" t="n">
+        <v>43831</v>
+      </c>
+      <c r="H8" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="I8" s="0" t="n">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G9" s="4" t="n">
+        <v>43831</v>
+      </c>
+      <c r="H9" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="I9" s="0" t="n">
         <v>32</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Add Product For the Child and Company Field
</commit_message>
<xml_diff>
--- a/ProductHistorical_TestData.xlsx
+++ b/ProductHistorical_TestData.xlsx
@@ -55,10 +55,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="3">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="GENERAL"/>
     <numFmt numFmtId="165" formatCode="DD/MM/YY"/>
-    <numFmt numFmtId="166" formatCode="DD/MM/YY"/>
   </numFmts>
   <fonts count="5">
     <font>
@@ -134,7 +133,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -148,10 +147,6 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -230,7 +225,7 @@
   <dimension ref="A1:R9"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I19" activeCellId="0" sqref="I19"/>
+      <selection pane="topLeft" activeCell="I4" activeCellId="0" sqref="I4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -247,7 +242,7 @@
     <col collapsed="false" hidden="false" max="1025" min="10" style="0" width="8.36296296296296"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="16.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
         <v>0</v>
       </c>
@@ -274,6 +269,9 @@
       </c>
       <c r="I1" s="0" t="n">
         <v>10</v>
+      </c>
+      <c r="J1" s="0" t="n">
+        <v>20</v>
       </c>
       <c r="K1" s="0" t="n">
         <v>30</v>
@@ -290,6 +288,9 @@
       <c r="I2" s="0" t="n">
         <v>11</v>
       </c>
+      <c r="J2" s="0" t="n">
+        <v>21</v>
+      </c>
       <c r="K2" s="0" t="n">
         <v>31</v>
       </c>
@@ -304,74 +305,95 @@
       <c r="I3" s="0" t="n">
         <v>12</v>
       </c>
+      <c r="J3" s="0" t="n">
+        <v>22</v>
+      </c>
       <c r="K3" s="0" t="n">
         <v>32</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="G4" s="4" t="n">
+      <c r="G4" s="3" t="n">
         <v>43276.5385855949</v>
       </c>
       <c r="H4" s="3" t="s">
         <v>8</v>
       </c>
       <c r="I4" s="0" t="n">
-        <v>20</v>
+        <v>13</v>
+      </c>
+      <c r="J4" s="0" t="n">
+        <v>23</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="G5" s="4" t="n">
+      <c r="G5" s="3" t="n">
         <v>43276.5385094428</v>
       </c>
       <c r="H5" s="0" t="s">
         <v>9</v>
       </c>
       <c r="I5" s="0" t="n">
-        <v>21</v>
+        <v>14</v>
+      </c>
+      <c r="J5" s="0" t="n">
+        <v>24</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="G6" s="4" t="n">
+      <c r="G6" s="3" t="n">
         <v>43276.5385244457</v>
       </c>
       <c r="H6" s="0" t="s">
         <v>10</v>
       </c>
       <c r="I6" s="0" t="n">
-        <v>22</v>
+        <v>15</v>
+      </c>
+      <c r="J6" s="0" t="n">
+        <v>25</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="G7" s="4" t="n">
+      <c r="G7" s="3" t="n">
         <v>43831</v>
       </c>
       <c r="H7" s="3" t="s">
         <v>8</v>
       </c>
       <c r="I7" s="0" t="n">
-        <v>30</v>
+        <v>16</v>
+      </c>
+      <c r="J7" s="0" t="n">
+        <v>26</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="G8" s="4" t="n">
+      <c r="G8" s="3" t="n">
         <v>43831</v>
       </c>
       <c r="H8" s="0" t="s">
         <v>9</v>
       </c>
       <c r="I8" s="0" t="n">
-        <v>31</v>
+        <v>17</v>
+      </c>
+      <c r="J8" s="0" t="n">
+        <v>27</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="G9" s="4" t="n">
+      <c r="G9" s="3" t="n">
         <v>43831</v>
       </c>
       <c r="H9" s="0" t="s">
         <v>10</v>
       </c>
       <c r="I9" s="0" t="n">
-        <v>32</v>
+        <v>18</v>
+      </c>
+      <c r="J9" s="0" t="n">
+        <v>28</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add the Customer for the Test
</commit_message>
<xml_diff>
--- a/ProductHistorical_TestData.xlsx
+++ b/ProductHistorical_TestData.xlsx
@@ -10,13 +10,14 @@
   <sheets>
     <sheet name="AddCurrency" sheetId="1" state="visible" r:id="rId2"/>
     <sheet name="AddProductCategory1" sheetId="2" state="visible" r:id="rId3"/>
+    <sheet name="AddCustomer" sheetId="3" state="visible" r:id="rId4"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="23">
   <si>
     <t>admin</t>
   </si>
@@ -42,13 +43,49 @@
     <t>Test Product1</t>
   </si>
   <si>
+    <t>'01/01/1970'</t>
+  </si>
+  <si>
     <t>United States Dollar</t>
   </si>
   <si>
+    <t>Test Product2</t>
+  </si>
+  <si>
     <t>Canadian Dollar</t>
   </si>
   <si>
+    <t>Test Product3</t>
+  </si>
+  <si>
     <t>Euro</t>
+  </si>
+  <si>
+    <t>Test Product4</t>
+  </si>
+  <si>
+    <t>'06/26/2018'</t>
+  </si>
+  <si>
+    <t>06/26/2018</t>
+  </si>
+  <si>
+    <t>'01/01/2020'</t>
+  </si>
+  <si>
+    <t>Default</t>
+  </si>
+  <si>
+    <t>USD Customer</t>
+  </si>
+  <si>
+    <t>CAD Customer</t>
+  </si>
+  <si>
+    <t>Canadian Dollar </t>
+  </si>
+  <si>
+    <t>Euro Customer</t>
   </si>
 </sst>
 </file>
@@ -133,7 +170,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -146,8 +183,12 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -170,7 +211,7 @@
   <dimension ref="A1:F1"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="F1" activeCellId="0" sqref="F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -225,7 +266,7 @@
   <dimension ref="A1:R9"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I4" activeCellId="0" sqref="I4"/>
+      <selection pane="topLeft" activeCell="H15" activeCellId="0" sqref="H15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -236,164 +277,320 @@
     <col collapsed="false" hidden="false" max="4" min="4" style="0" width="11.4592592592593"/>
     <col collapsed="false" hidden="false" max="5" min="5" style="0" width="18.9777777777778"/>
     <col collapsed="false" hidden="false" max="6" min="6" style="0" width="11.4592592592593"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="9.25555555555556"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="12.0074074074074"/>
     <col collapsed="false" hidden="false" max="8" min="8" style="0" width="16.8666666666667"/>
     <col collapsed="false" hidden="false" max="9" min="9" style="0" width="4.85555555555556"/>
     <col collapsed="false" hidden="false" max="1025" min="10" style="0" width="8.36296296296296"/>
   </cols>
   <sheetData>
+    <row r="1" customFormat="false" ht="16.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="I1" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="J1" s="0" t="n">
+        <v>20</v>
+      </c>
+      <c r="K1" s="0" t="n">
+        <v>30</v>
+      </c>
+      <c r="L1" s="0" t="n">
+        <v>40</v>
+      </c>
+      <c r="M1" s="0" t="n">
+        <v>50</v>
+      </c>
+      <c r="R1" s="3"/>
+    </row>
+    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F2" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="H2" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="I2" s="0" t="n">
+        <v>11</v>
+      </c>
+      <c r="J2" s="0" t="n">
+        <v>21</v>
+      </c>
+      <c r="K2" s="0" t="n">
+        <v>31</v>
+      </c>
+      <c r="L2" s="0" t="n">
+        <v>41</v>
+      </c>
+      <c r="M2" s="0" t="n">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F3" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="H3" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="I3" s="0" t="n">
+        <v>12</v>
+      </c>
+      <c r="J3" s="0" t="n">
+        <v>22</v>
+      </c>
+      <c r="K3" s="0" t="n">
+        <v>32</v>
+      </c>
+      <c r="L3" s="0" t="n">
+        <v>42</v>
+      </c>
+      <c r="M3" s="0" t="n">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F4" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="G4" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="H4" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="I4" s="0" t="n">
+        <v>13</v>
+      </c>
+      <c r="J4" s="0" t="n">
+        <v>23</v>
+      </c>
+      <c r="K4" s="0" t="n">
+        <v>33</v>
+      </c>
+      <c r="L4" s="0" t="n">
+        <v>43</v>
+      </c>
+      <c r="M4" s="0" t="n">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G5" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="H5" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="I5" s="0" t="n">
+        <v>14</v>
+      </c>
+      <c r="J5" s="0" t="n">
+        <v>24</v>
+      </c>
+      <c r="K5" s="0" t="n">
+        <v>34</v>
+      </c>
+      <c r="L5" s="0" t="n">
+        <v>44</v>
+      </c>
+      <c r="M5" s="0" t="n">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G6" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="H6" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="I6" s="0" t="n">
+        <v>15</v>
+      </c>
+      <c r="J6" s="0" t="n">
+        <v>25</v>
+      </c>
+      <c r="K6" s="0" t="n">
+        <v>35</v>
+      </c>
+      <c r="L6" s="0" t="n">
+        <v>45</v>
+      </c>
+      <c r="M6" s="0" t="n">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G7" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="H7" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="I7" s="0" t="n">
+        <v>16</v>
+      </c>
+      <c r="J7" s="0" t="n">
+        <v>26</v>
+      </c>
+      <c r="K7" s="0" t="n">
+        <v>36</v>
+      </c>
+      <c r="L7" s="0" t="n">
+        <v>46</v>
+      </c>
+      <c r="M7" s="0" t="n">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G8" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="H8" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="I8" s="0" t="n">
+        <v>17</v>
+      </c>
+      <c r="J8" s="0" t="n">
+        <v>27</v>
+      </c>
+      <c r="K8" s="0" t="n">
+        <v>37</v>
+      </c>
+      <c r="L8" s="0" t="n">
+        <v>47</v>
+      </c>
+      <c r="M8" s="0" t="n">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G9" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="H9" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="I9" s="0" t="n">
+        <v>18</v>
+      </c>
+      <c r="J9" s="0" t="n">
+        <v>28</v>
+      </c>
+      <c r="K9" s="0" t="n">
+        <v>38</v>
+      </c>
+      <c r="L9" s="0" t="n">
+        <v>48</v>
+      </c>
+      <c r="M9" s="0" t="n">
+        <v>58</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B1" r:id="rId1" display="WebData@123"/>
+  </hyperlinks>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:F3"/>
+  <sheetViews>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D1" activeCellId="0" sqref="D1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.36296296296296"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="12.9296296296296"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="18.8851851851852"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="7.97777777777778"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="12.7407407407407"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="18.8851851851852"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="8.36296296296296"/>
+  </cols>
+  <sheetData>
     <row r="1" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="0" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="0" t="s">
         <v>2</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>6</v>
+        <v>18</v>
       </c>
       <c r="E1" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C2" s="0" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="0" t="s">
-        <v>7</v>
-      </c>
-      <c r="G1" s="3" t="n">
-        <v>25569</v>
-      </c>
-      <c r="H1" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="I1" s="0" t="n">
-        <v>10</v>
-      </c>
-      <c r="J1" s="0" t="n">
+      <c r="E2" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="K1" s="0" t="n">
-        <v>30</v>
-      </c>
-      <c r="R1" s="3"/>
-    </row>
-    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="G2" s="3" t="n">
-        <v>25569</v>
-      </c>
-      <c r="H2" s="0" t="s">
-        <v>9</v>
-      </c>
-      <c r="I2" s="0" t="n">
-        <v>11</v>
-      </c>
-      <c r="J2" s="0" t="n">
+      <c r="F2" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="K2" s="0" t="n">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="G3" s="3" t="n">
-        <v>25569</v>
-      </c>
-      <c r="H3" s="0" t="s">
-        <v>10</v>
-      </c>
-      <c r="I3" s="0" t="n">
-        <v>12</v>
-      </c>
-      <c r="J3" s="0" t="n">
+    </row>
+    <row r="3" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E3" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="K3" s="0" t="n">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="G4" s="3" t="n">
-        <v>43276.5385855949</v>
-      </c>
-      <c r="H4" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="I4" s="0" t="n">
+      <c r="F3" s="4" t="s">
         <v>13</v>
-      </c>
-      <c r="J4" s="0" t="n">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="G5" s="3" t="n">
-        <v>43276.5385094428</v>
-      </c>
-      <c r="H5" s="0" t="s">
-        <v>9</v>
-      </c>
-      <c r="I5" s="0" t="n">
-        <v>14</v>
-      </c>
-      <c r="J5" s="0" t="n">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="G6" s="3" t="n">
-        <v>43276.5385244457</v>
-      </c>
-      <c r="H6" s="0" t="s">
-        <v>10</v>
-      </c>
-      <c r="I6" s="0" t="n">
-        <v>15</v>
-      </c>
-      <c r="J6" s="0" t="n">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="G7" s="3" t="n">
-        <v>43831</v>
-      </c>
-      <c r="H7" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="I7" s="0" t="n">
-        <v>16</v>
-      </c>
-      <c r="J7" s="0" t="n">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="G8" s="3" t="n">
-        <v>43831</v>
-      </c>
-      <c r="H8" s="0" t="s">
-        <v>9</v>
-      </c>
-      <c r="I8" s="0" t="n">
-        <v>17</v>
-      </c>
-      <c r="J8" s="0" t="n">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="G9" s="3" t="n">
-        <v>43831</v>
-      </c>
-      <c r="H9" s="0" t="s">
-        <v>10</v>
-      </c>
-      <c r="I9" s="0" t="n">
-        <v>18</v>
-      </c>
-      <c r="J9" s="0" t="n">
-        <v>28</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Complete Product Historical Feature Code
</commit_message>
<xml_diff>
--- a/ProductHistorical_TestData.xlsx
+++ b/ProductHistorical_TestData.xlsx
@@ -5,19 +5,20 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="927" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="927" firstSheet="0" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="AddCurrency" sheetId="1" state="visible" r:id="rId2"/>
     <sheet name="AddProductCategory1" sheetId="2" state="visible" r:id="rId3"/>
     <sheet name="AddCustomer" sheetId="3" state="visible" r:id="rId4"/>
+    <sheet name="CreateOrder" sheetId="4" state="visible" r:id="rId5"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="23">
   <si>
     <t>admin</t>
   </si>
@@ -25,16 +26,16 @@
     <t>WebData@123</t>
   </si>
   <si>
-    <t>Web Data Sanity</t>
-  </si>
-  <si>
-    <t>Web Data Sanity Child</t>
+    <t>Sanity Suite Test</t>
+  </si>
+  <si>
+    <t>Sanity Suite Test Child</t>
   </si>
   <si>
     <t>Currencies updated successfully.</t>
   </si>
   <si>
-    <t>Working as admin Web Data Sanity Child X</t>
+    <t>Working as admin Sanity Suite Test Child X</t>
   </si>
   <si>
     <t>Test Category</t>
@@ -82,10 +83,10 @@
     <t>CAD Customer</t>
   </si>
   <si>
-    <t>Canadian Dollar </t>
-  </si>
-  <si>
     <t>Euro Customer</t>
+  </si>
+  <si>
+    <t>'01/26/2017'</t>
   </si>
 </sst>
 </file>
@@ -211,7 +212,7 @@
   <dimension ref="A1:F1"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F1" activeCellId="0" sqref="F1"/>
+      <selection pane="topLeft" activeCell="F1" activeCellId="1" sqref="C1:C2 F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -265,8 +266,8 @@
   </sheetPr>
   <dimension ref="A1:R9"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H15" activeCellId="0" sqref="H15"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G9" activeCellId="1" sqref="C1:C2 G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -540,7 +541,7 @@
   <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D1" activeCellId="0" sqref="D1"/>
+      <selection pane="topLeft" activeCell="E1" activeCellId="1" sqref="C1:C2 E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -582,15 +583,187 @@
         <v>20</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>21</v>
+        <v>11</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E3" s="4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F3" s="4" t="s">
         <v>13</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B1" r:id="rId1" display="WebData@123"/>
+  </hyperlinks>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:M4"/>
+  <sheetViews>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E10" activeCellId="1" sqref="C1:C2 E10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.36296296296296"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="13.3851851851852"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="18.8851851851852"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="12.7407407407407"/>
+    <col collapsed="false" hidden="false" max="7" min="5" style="0" width="11.4592592592593"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="4.02962962962963"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="4.3037037037037"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="3.84814814814815"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="3.94074074074074"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="4.3037037037037"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="3.94074074074074"/>
+    <col collapsed="false" hidden="false" max="1025" min="14" style="0" width="8.36296296296296"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="0" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="F1" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="G1" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="H1" s="4" t="n">
+        <v>90</v>
+      </c>
+      <c r="I1" s="4" t="n">
+        <v>120</v>
+      </c>
+      <c r="J1" s="4" t="n">
+        <v>93</v>
+      </c>
+      <c r="K1" s="4" t="n">
+        <v>123</v>
+      </c>
+      <c r="L1" s="4" t="n">
+        <v>96</v>
+      </c>
+      <c r="M1" s="4" t="n">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C2" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="F2" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="G2" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="H2" s="4" t="n">
+        <v>90</v>
+      </c>
+      <c r="I2" s="4" t="n">
+        <v>120</v>
+      </c>
+      <c r="J2" s="4" t="n">
+        <v>93</v>
+      </c>
+      <c r="K2" s="4" t="n">
+        <v>123</v>
+      </c>
+      <c r="L2" s="4" t="n">
+        <v>96</v>
+      </c>
+      <c r="M2" s="4" t="n">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D3" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="F3" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="G3" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="H3" s="4" t="n">
+        <v>99</v>
+      </c>
+      <c r="I3" s="4" t="n">
+        <v>129</v>
+      </c>
+      <c r="J3" s="4" t="n">
+        <v>102</v>
+      </c>
+      <c r="K3" s="4" t="n">
+        <v>132</v>
+      </c>
+      <c r="L3" s="4" t="n">
+        <v>105</v>
+      </c>
+      <c r="M3" s="4" t="n">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E4" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="H4" s="4" t="n">
+        <v>108</v>
+      </c>
+      <c r="I4" s="4" t="n">
+        <v>138</v>
+      </c>
+      <c r="J4" s="4" t="n">
+        <v>111</v>
+      </c>
+      <c r="K4" s="4" t="n">
+        <v>141</v>
+      </c>
+      <c r="L4" s="4" t="n">
+        <v>114</v>
+      </c>
+      <c r="M4" s="4" t="n">
+        <v>144</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
code changes for product historical features
</commit_message>
<xml_diff>
--- a/ProductHistorical_TestData.xlsx
+++ b/ProductHistorical_TestData.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="LoginSignup" sheetId="1" state="visible" r:id="rId2"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="36">
   <si>
     <t xml:space="preserve">admin</t>
   </si>
@@ -32,7 +32,7 @@
     <t xml:space="preserve">WebData@123</t>
   </si>
   <si>
-    <t xml:space="preserve">Web Data 59</t>
+    <t xml:space="preserve">Web Data 60</t>
   </si>
   <si>
     <t xml:space="preserve">Marta</t>
@@ -59,7 +59,7 @@
     <t xml:space="preserve">United States Dollar</t>
   </si>
   <si>
-    <t xml:space="preserve">Child Web Data 59</t>
+    <t xml:space="preserve">Child Web Data 60</t>
   </si>
   <si>
     <t xml:space="preserve">H-50</t>
@@ -77,19 +77,13 @@
     <t xml:space="preserve">301520</t>
   </si>
   <si>
-    <t xml:space="preserve">Successfully created Child Web Data 59. You can now login with the username admin after your password is set. Password reset link is sent to your email.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Web Data 58</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Web Data 58 Child</t>
+    <t xml:space="preserve">Successfully created Child Web Data 60. You can now login with the username admin after your password is set. Password reset link is sent to your email.</t>
   </si>
   <si>
     <t xml:space="preserve">Currencies updated successfully.</t>
   </si>
   <si>
-    <t xml:space="preserve">Working as admin Web Data 58 Child X</t>
+    <t xml:space="preserve">Working as admin Child Web Data 60 X</t>
   </si>
   <si>
     <t xml:space="preserve">Test Category</t>
@@ -336,18 +330,18 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:U1"/>
+  <dimension ref="1:1"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D16" activeCellId="0" sqref="D16"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E1" activeCellId="0" sqref="E1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.52592592592593"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.81851851851852"/>
   </cols>
   <sheetData>
-    <row r="1" s="1" customFormat="true" ht="15.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" s="1" customFormat="true" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -411,6 +405,7 @@
       <c r="U1" s="1" t="s">
         <v>17</v>
       </c>
+      <c r="AMJ1" s="0"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -436,18 +431,18 @@
   <dimension ref="A1:F1"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="C1" activeCellId="0" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="9.6037037037037"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="13.5222222222222"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="16.8555555555556"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="23.6148148148148"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="29.1037037037037"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="38.4148148148148"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="1" width="9.6037037037037"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="9.9962962962963"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="14.1111111111111"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="17.6407407407407"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="24.7925925925926"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="30.5740740740741"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="40.3740740740741"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="1" width="9.9962962962963"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -458,16 +453,16 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>19</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>21</v>
       </c>
     </row>
   </sheetData>
@@ -492,24 +487,24 @@
   <dimension ref="A1:R9"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G9" activeCellId="0" sqref="G9"/>
+      <selection pane="topLeft" activeCell="E1" activeCellId="0" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="7.44814814814815"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="9.01481481481481"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="16.462962962963"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="12.4444444444444"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="20.8740740740741"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="12.4444444444444"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="12.837037037037"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="18.4222222222222"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="5.29259259259259"/>
-    <col collapsed="false" hidden="false" max="1025" min="10" style="1" width="9.01481481481481"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="7.64444444444445"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="9.40740740740741"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="17.2481481481481"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="12.837037037037"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="21.9518518518519"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="12.837037037037"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="13.4259259259259"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="19.2074074074074"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="5.48888888888889"/>
+    <col collapsed="false" hidden="false" max="1025" min="10" style="1" width="9.40740740740741"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="16.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -517,19 +512,19 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>18</v>
+        <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="G1" s="4" t="s">
         <v>22</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="G1" s="4" t="s">
-        <v>24</v>
       </c>
       <c r="H1" s="4" t="s">
         <v>10</v>
@@ -553,13 +548,13 @@
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F2" s="1" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="G2" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="H2" s="1" t="s">
         <v>24</v>
-      </c>
-      <c r="H2" s="1" t="s">
-        <v>26</v>
       </c>
       <c r="I2" s="1" t="n">
         <v>11</v>
@@ -579,13 +574,13 @@
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F3" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="G3" s="4" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="I3" s="1" t="n">
         <v>12</v>
@@ -605,10 +600,10 @@
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F4" s="1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="G4" s="4" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="H4" s="4" t="s">
         <v>10</v>
@@ -631,10 +626,10 @@
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="G5" s="4" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="I5" s="1" t="n">
         <v>14</v>
@@ -654,10 +649,10 @@
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="G6" s="4" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="I6" s="1" t="n">
         <v>15</v>
@@ -677,7 +672,7 @@
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="G7" s="4" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="H7" s="4" t="s">
         <v>10</v>
@@ -700,10 +695,10 @@
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="G8" s="4" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="I8" s="1" t="n">
         <v>17</v>
@@ -723,10 +718,10 @@
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="G9" s="4" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="I9" s="1" t="n">
         <v>18</v>
@@ -766,18 +761,18 @@
   <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E3" activeCellId="0" sqref="E3"/>
+      <selection pane="topLeft" activeCell="D1" activeCellId="0" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="9.01481481481481"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="14.1111111111111"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="20.7740740740741"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="8.42592592592593"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="13.8185185185185"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="20.7740740740741"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="1" width="9.01481481481481"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="9.40740740740741"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="14.7"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="21.8518518518519"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="8.62222222222222"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="14.4037037037037"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="21.8518518518519"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="1" width="9.40740740740741"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -788,13 +783,13 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>18</v>
+        <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="F1" s="5" t="s">
         <v>10</v>
@@ -802,21 +797,21 @@
     </row>
     <row r="2" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C2" s="1" t="s">
-        <v>19</v>
+        <v>11</v>
       </c>
       <c r="E2" s="5" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="F2" s="5" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E3" s="5" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="F3" s="5" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
   </sheetData>
@@ -840,24 +835,24 @@
   </sheetPr>
   <dimension ref="A1:M4"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E10" activeCellId="0" sqref="E10"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="9.01481481481481"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="14.6"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="20.7740740740741"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="13.8185185185185"/>
-    <col collapsed="false" hidden="false" max="7" min="5" style="1" width="12.4444444444444"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="9.40740740740741"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="15.2888888888889"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="21.8518518518519"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="14.4037037037037"/>
+    <col collapsed="false" hidden="false" max="7" min="5" style="1" width="12.837037037037"/>
     <col collapsed="false" hidden="false" max="8" min="8" style="1" width="4.01851851851852"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="4.7037037037037"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="4.9"/>
     <col collapsed="false" hidden="false" max="10" min="10" style="1" width="3.82222222222222"/>
     <col collapsed="false" hidden="false" max="11" min="11" style="1" width="3.91851851851852"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="1" width="4.7037037037037"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="1" width="4.9"/>
     <col collapsed="false" hidden="false" max="13" min="13" style="1" width="3.91851851851852"/>
-    <col collapsed="false" hidden="false" max="1025" min="14" style="1" width="9.01481481481481"/>
+    <col collapsed="false" hidden="false" max="1025" min="14" style="1" width="9.40740740740741"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -868,19 +863,19 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>18</v>
+        <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="E1" s="4" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="H1" s="5" t="n">
         <v>90</v>
@@ -903,19 +898,19 @@
     </row>
     <row r="2" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C2" s="1" t="s">
-        <v>19</v>
+        <v>11</v>
       </c>
       <c r="D2" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="E2" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="E2" s="4" t="s">
-        <v>37</v>
-      </c>
       <c r="F2" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="G2" s="1" t="s">
         <v>25</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>27</v>
       </c>
       <c r="H2" s="5" t="n">
         <v>90</v>
@@ -938,16 +933,16 @@
     </row>
     <row r="3" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D3" s="5" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="H3" s="5" t="n">
         <v>99</v>
@@ -970,7 +965,7 @@
     </row>
     <row r="4" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E4" s="4" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="H4" s="5" t="n">
         <v>108</v>

</xml_diff>

<commit_message>
Code Changes for the Parent comoany customers
</commit_message>
<xml_diff>
--- a/ProductHistorical_TestData.xlsx
+++ b/ProductHistorical_TestData.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="37">
   <si>
     <t xml:space="preserve">admin</t>
   </si>
@@ -132,6 +132,9 @@
   </si>
   <si>
     <t xml:space="preserve">'01/26/2017'</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Working as admin Child Web Data 60 X</t>
   </si>
 </sst>
 </file>
@@ -836,14 +839,14 @@
   <dimension ref="A1:M4"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
+      <selection pane="topLeft" activeCell="C3" activeCellId="0" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="1" width="9.40740740740741"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="1" width="15.2888888888889"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="21.8518518518519"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="34.2925925925926"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="1" width="14.4037037037037"/>
     <col collapsed="false" hidden="false" max="7" min="5" style="1" width="12.837037037037"/>
     <col collapsed="false" hidden="false" max="8" min="8" style="1" width="4.01851851851852"/>
@@ -932,6 +935,9 @@
       </c>
     </row>
     <row r="3" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C3" s="5" t="s">
+        <v>36</v>
+      </c>
       <c r="D3" s="5" t="s">
         <v>34</v>
       </c>

</xml_diff>

<commit_message>
Complete Code Changes For Product Historical Price Feature Test Plan
</commit_message>
<xml_diff>
--- a/ProductHistorical_TestData.xlsx
+++ b/ProductHistorical_TestData.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="46">
   <si>
     <t xml:space="preserve">admin</t>
   </si>
@@ -32,7 +32,7 @@
     <t xml:space="preserve">WebData@123</t>
   </si>
   <si>
-    <t xml:space="preserve">Web Data 60</t>
+    <t xml:space="preserve">Web Data 64</t>
   </si>
   <si>
     <t xml:space="preserve">Marta</t>
@@ -59,7 +59,7 @@
     <t xml:space="preserve">United States Dollar</t>
   </si>
   <si>
-    <t xml:space="preserve">Child Web Data 60</t>
+    <t xml:space="preserve">Child Web Data 64</t>
   </si>
   <si>
     <t xml:space="preserve">H-50</t>
@@ -77,13 +77,13 @@
     <t xml:space="preserve">301520</t>
   </si>
   <si>
-    <t xml:space="preserve">Successfully created Child Web Data 60. You can now login with the username admin after your password is set. Password reset link is sent to your email.</t>
+    <t xml:space="preserve">Successfully created Child Web Data 64. You can now login with the username admin after your password is set. Password reset link is sent to your email.</t>
   </si>
   <si>
     <t xml:space="preserve">Currencies updated successfully.</t>
   </si>
   <si>
-    <t xml:space="preserve">Working as admin Child Web Data 60 X</t>
+    <t xml:space="preserve">Working as admin Child Web Data 64 X</t>
   </si>
   <si>
     <t xml:space="preserve">Test Category</t>
@@ -131,10 +131,37 @@
     <t xml:space="preserve">Euro Customer</t>
   </si>
   <si>
+    <t xml:space="preserve">Total = US$90.00</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Total = US$120.00</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Total = C$93.00</t>
+  </si>
+  <si>
     <t xml:space="preserve">'01/26/2017'</t>
   </si>
   <si>
-    <t xml:space="preserve">Working as admin Child Web Data 60 X</t>
+    <t xml:space="preserve">Working as admin Child Web Data 64 X</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Total = US$99.00</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Total = US$129.00</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Total = C$102.00</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Total = US$108.00</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Total = US$138.00</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Total = C$111.00</t>
   </si>
 </sst>
 </file>
@@ -145,7 +172,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="DD/MM/YY"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="7">
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
@@ -183,6 +210,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -230,7 +263,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -252,6 +285,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -336,12 +373,12 @@
   <dimension ref="1:1"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E1" activeCellId="0" sqref="E1"/>
+      <selection pane="topLeft" activeCell="N1" activeCellId="0" sqref="N1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.81851851851852"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="9.01481481481481"/>
   </cols>
   <sheetData>
     <row r="1" s="1" customFormat="true" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -434,18 +471,18 @@
   <dimension ref="A1:F1"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C1" activeCellId="0" sqref="C1"/>
+      <selection pane="topLeft" activeCell="G1" activeCellId="0" sqref="G1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="9.9962962962963"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="14.1111111111111"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="17.6407407407407"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="24.7925925925926"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="30.5740740740741"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="40.3740740740741"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="1" width="9.9962962962963"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="10.1925925925926"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="14.4037037037037"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="18.0296296296296"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="25.3814814814815"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="31.3592592592593"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="41.3518518518519"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="1" width="10.1925925925926"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -489,22 +526,22 @@
   </sheetPr>
   <dimension ref="A1:R9"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E1" activeCellId="0" sqref="E1"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="O1" activeCellId="0" sqref="O1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="7.64444444444445"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="9.40740740740741"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="17.2481481481481"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="12.837037037037"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="21.9518518518519"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="12.837037037037"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="13.4259259259259"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="19.2074074074074"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="5.48888888888889"/>
-    <col collapsed="false" hidden="false" max="1025" min="10" style="1" width="9.40740740740741"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="7.74074074074074"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="9.6037037037037"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="17.6407407407407"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="13.1296296296296"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="22.4407407407407"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="13.1296296296296"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="13.7185185185185"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="19.6962962962963"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="5.58518518518519"/>
+    <col collapsed="false" hidden="false" max="1025" min="10" style="1" width="9.6037037037037"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -547,6 +584,9 @@
       <c r="M1" s="1" t="n">
         <v>50</v>
       </c>
+      <c r="N1" s="1" t="n">
+        <v>60</v>
+      </c>
       <c r="R1" s="4"/>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -574,6 +614,9 @@
       <c r="M2" s="1" t="n">
         <v>51</v>
       </c>
+      <c r="N2" s="1" t="n">
+        <v>61</v>
+      </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F3" s="1" t="s">
@@ -600,6 +643,9 @@
       <c r="M3" s="1" t="n">
         <v>52</v>
       </c>
+      <c r="N3" s="1" t="n">
+        <v>62</v>
+      </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F4" s="1" t="s">
@@ -626,6 +672,9 @@
       <c r="M4" s="1" t="n">
         <v>53</v>
       </c>
+      <c r="N4" s="1" t="n">
+        <v>63</v>
+      </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="G5" s="4" t="s">
@@ -649,6 +698,9 @@
       <c r="M5" s="1" t="n">
         <v>54</v>
       </c>
+      <c r="N5" s="1" t="n">
+        <v>64</v>
+      </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="G6" s="4" t="s">
@@ -672,6 +724,9 @@
       <c r="M6" s="1" t="n">
         <v>55</v>
       </c>
+      <c r="N6" s="1" t="n">
+        <v>65</v>
+      </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="G7" s="4" t="s">
@@ -695,6 +750,9 @@
       <c r="M7" s="1" t="n">
         <v>56</v>
       </c>
+      <c r="N7" s="1" t="n">
+        <v>66</v>
+      </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="G8" s="4" t="s">
@@ -718,6 +776,9 @@
       <c r="M8" s="1" t="n">
         <v>57</v>
       </c>
+      <c r="N8" s="1" t="n">
+        <v>67</v>
+      </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="G9" s="4" t="s">
@@ -740,6 +801,9 @@
       </c>
       <c r="M9" s="1" t="n">
         <v>58</v>
+      </c>
+      <c r="N9" s="1" t="n">
+        <v>68</v>
       </c>
     </row>
   </sheetData>
@@ -764,18 +828,18 @@
   <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D1" activeCellId="0" sqref="D1"/>
+      <selection pane="topLeft" activeCell="E1" activeCellId="0" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="9.40740740740741"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="14.7"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="21.8518518518519"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="8.62222222222222"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="14.4037037037037"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="21.8518518518519"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="1" width="9.40740740740741"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="9.6037037037037"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="14.9925925925926"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="22.3444444444444"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="8.81851851851852"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="14.7"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="22.3444444444444"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="1" width="9.6037037037037"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -839,26 +903,26 @@
   <dimension ref="A1:M4"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C3" activeCellId="0" sqref="C3"/>
+      <selection pane="topLeft" activeCell="I5" activeCellId="0" sqref="I5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="9.40740740740741"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="15.2888888888889"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="34.2925925925926"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="14.4037037037037"/>
-    <col collapsed="false" hidden="false" max="7" min="5" style="1" width="12.837037037037"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="4.01851851851852"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="4.9"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="3.82222222222222"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="9.6037037037037"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="15.6777777777778"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="35.1814814814815"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="14.7"/>
+    <col collapsed="false" hidden="false" max="7" min="5" style="1" width="13.1296296296296"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="18.6111111111111"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="23.4740740740741"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="20.1666666666667"/>
     <col collapsed="false" hidden="false" max="11" min="11" style="1" width="3.91851851851852"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="1" width="4.9"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="1" width="4.9962962962963"/>
     <col collapsed="false" hidden="false" max="13" min="13" style="1" width="3.91851851851852"/>
-    <col collapsed="false" hidden="false" max="1025" min="14" style="1" width="9.40740740740741"/>
+    <col collapsed="false" hidden="false" max="1025" min="14" style="1" width="9.6037037037037"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="20.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -880,14 +944,14 @@
       <c r="G1" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="H1" s="5" t="n">
-        <v>90</v>
-      </c>
-      <c r="I1" s="5" t="n">
-        <v>120</v>
-      </c>
-      <c r="J1" s="5" t="n">
-        <v>93</v>
+      <c r="H1" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="I1" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="J1" s="5" t="s">
+        <v>37</v>
       </c>
       <c r="K1" s="5" t="n">
         <v>123</v>
@@ -907,7 +971,7 @@
         <v>33</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="F2" s="1" t="s">
         <v>23</v>
@@ -915,14 +979,14 @@
       <c r="G2" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="H2" s="5" t="n">
-        <v>90</v>
-      </c>
-      <c r="I2" s="5" t="n">
-        <v>120</v>
-      </c>
-      <c r="J2" s="5" t="n">
-        <v>93</v>
+      <c r="H2" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="I2" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="J2" s="5" t="s">
+        <v>37</v>
       </c>
       <c r="K2" s="5" t="n">
         <v>123</v>
@@ -936,7 +1000,7 @@
     </row>
     <row r="3" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C3" s="5" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="D3" s="5" t="s">
         <v>34</v>
@@ -950,14 +1014,14 @@
       <c r="G3" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="H3" s="5" t="n">
-        <v>99</v>
-      </c>
-      <c r="I3" s="5" t="n">
-        <v>129</v>
-      </c>
-      <c r="J3" s="5" t="n">
-        <v>102</v>
+      <c r="H3" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="I3" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="J3" s="5" t="s">
+        <v>42</v>
       </c>
       <c r="K3" s="5" t="n">
         <v>132</v>
@@ -973,14 +1037,14 @@
       <c r="E4" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="H4" s="5" t="n">
-        <v>108</v>
-      </c>
-      <c r="I4" s="5" t="n">
-        <v>138</v>
-      </c>
-      <c r="J4" s="5" t="n">
-        <v>111</v>
+      <c r="H4" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="I4" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="J4" s="5" t="s">
+        <v>45</v>
       </c>
       <c r="K4" s="5" t="n">
         <v>141</v>

</xml_diff>

<commit_message>
makes relative xpath in productHistorical package
</commit_message>
<xml_diff>
--- a/ProductHistorical_TestData.xlsx
+++ b/ProductHistorical_TestData.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="59">
   <si>
     <t xml:space="preserve">admin</t>
   </si>
@@ -32,7 +32,7 @@
     <t xml:space="preserve">WebData@123</t>
   </si>
   <si>
-    <t xml:space="preserve">Web Data 64</t>
+    <t xml:space="preserve">Web Data 33</t>
   </si>
   <si>
     <t xml:space="preserve">Marta</t>
@@ -59,7 +59,7 @@
     <t xml:space="preserve">United States Dollar</t>
   </si>
   <si>
-    <t xml:space="preserve">Child Web Data 64</t>
+    <t xml:space="preserve">Child Web Data 33</t>
   </si>
   <si>
     <t xml:space="preserve">H-50</t>
@@ -77,13 +77,13 @@
     <t xml:space="preserve">301520</t>
   </si>
   <si>
-    <t xml:space="preserve">Successfully created Child Web Data 64. You can now login with the username admin after your password is set. Password reset link is sent to your email.</t>
+    <t xml:space="preserve">Successfully created Child Web Data 33. You can now login with the username admin after your password is set. Password reset link is sent to your email.</t>
   </si>
   <si>
     <t xml:space="preserve">Currencies updated successfully.</t>
   </si>
   <si>
-    <t xml:space="preserve">Working as admin Child Web Data 64 X</t>
+    <t xml:space="preserve">Working as admin Child Web Data 33 X</t>
   </si>
   <si>
     <t xml:space="preserve">Test Category</t>
@@ -131,6 +131,9 @@
     <t xml:space="preserve">Euro Customer</t>
   </si>
   <si>
+    <t xml:space="preserve">Test Product 1</t>
+  </si>
+  <si>
     <t xml:space="preserve">Total = US$90.00</t>
   </si>
   <si>
@@ -140,10 +143,28 @@
     <t xml:space="preserve">Total = C$93.00</t>
   </si>
   <si>
+    <t xml:space="preserve">Total = C$123.00</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Total = €96.00</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Total = €126.00</t>
+  </si>
+  <si>
     <t xml:space="preserve">'01/26/2017'</t>
   </si>
   <si>
-    <t xml:space="preserve">Working as admin Child Web Data 64 X</t>
+    <t xml:space="preserve">Test Product 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Test Product 3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Working as admin Child Web Data 33 X</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Test Product 4</t>
   </si>
   <si>
     <t xml:space="preserve">Total = US$99.00</t>
@@ -155,6 +176,15 @@
     <t xml:space="preserve">Total = C$102.00</t>
   </si>
   <si>
+    <t xml:space="preserve">Total = C$132.00</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Total = €105.00</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Total = €135.00</t>
+  </si>
+  <si>
     <t xml:space="preserve">Total = US$108.00</t>
   </si>
   <si>
@@ -162,6 +192,15 @@
   </si>
   <si>
     <t xml:space="preserve">Total = C$111.00</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Total = C$141.00</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Total = €114.00</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Total = €144.00</t>
   </si>
 </sst>
 </file>
@@ -172,7 +211,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="DD/MM/YY"/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="6">
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
@@ -210,12 +249,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -263,7 +296,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="6">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -285,10 +318,6 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -373,12 +402,12 @@
   <dimension ref="1:1"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="N1" activeCellId="0" sqref="N1"/>
+      <selection pane="topLeft" activeCell="D1" activeCellId="0" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="9.01481481481481"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="9.21111111111111"/>
   </cols>
   <sheetData>
     <row r="1" s="1" customFormat="true" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -471,18 +500,18 @@
   <dimension ref="A1:F1"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G1" activeCellId="0" sqref="G1"/>
+      <selection pane="topLeft" activeCell="C1" activeCellId="0" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="10.1925925925926"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="14.4037037037037"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="18.0296296296296"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="25.3814814814815"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="31.3592592592593"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="41.3518518518519"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="1" width="10.1925925925926"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="10.3888888888889"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="14.7"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="18.4222222222222"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="25.9666666666667"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="32.1407407407407"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="42.3333333333333"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="1" width="10.3888888888889"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -526,22 +555,22 @@
   </sheetPr>
   <dimension ref="A1:R9"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="O1" activeCellId="0" sqref="O1"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C1" activeCellId="0" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="7.74074074074074"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="9.6037037037037"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="17.6407407407407"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="13.1296296296296"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="22.4407407407407"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="13.1296296296296"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="13.7185185185185"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="19.6962962962963"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="5.58518518518519"/>
-    <col collapsed="false" hidden="false" max="1025" min="10" style="1" width="9.6037037037037"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="7.84074074074074"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="9.8"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="18.0296296296296"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="13.4259259259259"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="22.9296296296296"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="13.4259259259259"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="14.0148148148148"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="20.1851851851852"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="5.68518518518519"/>
+    <col collapsed="false" hidden="false" max="1025" min="10" style="1" width="9.8"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -828,18 +857,18 @@
   <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E1" activeCellId="0" sqref="E1"/>
+      <selection pane="topLeft" activeCell="C1" activeCellId="0" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="9.6037037037037"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="14.9925925925926"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="22.3444444444444"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="8.81851851851852"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="14.7"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="22.3444444444444"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="1" width="9.6037037037037"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="9.8"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="15.3851851851852"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="22.8333333333333"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="9.01481481481481"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="14.9925925925926"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="22.8333333333333"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="1" width="9.8"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -902,24 +931,24 @@
   </sheetPr>
   <dimension ref="A1:M4"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I5" activeCellId="0" sqref="I5"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="E1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="M5" activeCellId="0" sqref="M5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="9.6037037037037"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="15.6777777777778"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="35.1814814814815"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="14.7"/>
-    <col collapsed="false" hidden="false" max="7" min="5" style="1" width="13.1296296296296"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="18.6111111111111"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="23.4740740740741"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="20.1666666666667"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="1" width="3.91851851851852"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="1" width="4.9962962962963"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="1" width="3.91851851851852"/>
-    <col collapsed="false" hidden="false" max="1025" min="14" style="1" width="9.6037037037037"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="9.8"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="16.0703703703704"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="36.062962962963"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="14.9925925925926"/>
+    <col collapsed="false" hidden="false" max="7" min="5" style="1" width="13.4259259259259"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="19.0111111111111"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="24.1074074074074"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="20.6777777777778"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="1" width="17.4185185185185"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="1" width="13.6592592592593"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="1" width="16.9592592592593"/>
+    <col collapsed="false" hidden="false" max="1025" min="14" style="1" width="9.8"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="20.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -939,28 +968,28 @@
         <v>22</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>21</v>
+        <v>35</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>21</v>
+        <v>35</v>
       </c>
       <c r="H1" s="5" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="I1" s="5" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="J1" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="K1" s="5" t="n">
-        <v>123</v>
-      </c>
-      <c r="L1" s="5" t="n">
-        <v>96</v>
-      </c>
-      <c r="M1" s="5" t="n">
-        <v>126</v>
+        <v>38</v>
+      </c>
+      <c r="K1" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="L1" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="M1" s="5" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -971,36 +1000,36 @@
         <v>33</v>
       </c>
       <c r="E2" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="H2" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="I2" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="J2" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="F2" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="H2" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="I2" s="5" t="s">
-        <v>36</v>
-      </c>
-      <c r="J2" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="K2" s="5" t="n">
-        <v>123</v>
-      </c>
-      <c r="L2" s="5" t="n">
-        <v>96</v>
-      </c>
-      <c r="M2" s="5" t="n">
-        <v>126</v>
+      <c r="K2" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="L2" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="M2" s="5" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C3" s="5" t="s">
-        <v>39</v>
+        <v>45</v>
       </c>
       <c r="D3" s="5" t="s">
         <v>34</v>
@@ -1009,28 +1038,28 @@
         <v>28</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>27</v>
+        <v>46</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>27</v>
+        <v>46</v>
       </c>
       <c r="H3" s="5" t="s">
-        <v>40</v>
+        <v>47</v>
       </c>
       <c r="I3" s="5" t="s">
-        <v>41</v>
+        <v>48</v>
       </c>
       <c r="J3" s="5" t="s">
-        <v>42</v>
-      </c>
-      <c r="K3" s="5" t="n">
-        <v>132</v>
-      </c>
-      <c r="L3" s="5" t="n">
-        <v>105</v>
-      </c>
-      <c r="M3" s="5" t="n">
-        <v>135</v>
+        <v>49</v>
+      </c>
+      <c r="K3" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="L3" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="M3" s="5" t="s">
+        <v>52</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1038,22 +1067,22 @@
         <v>30</v>
       </c>
       <c r="H4" s="5" t="s">
-        <v>43</v>
+        <v>53</v>
       </c>
       <c r="I4" s="5" t="s">
-        <v>44</v>
+        <v>54</v>
       </c>
       <c r="J4" s="5" t="s">
-        <v>45</v>
-      </c>
-      <c r="K4" s="5" t="n">
-        <v>141</v>
-      </c>
-      <c r="L4" s="5" t="n">
-        <v>114</v>
-      </c>
-      <c r="M4" s="5" t="n">
-        <v>144</v>
+        <v>55</v>
+      </c>
+      <c r="K4" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="L4" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="M4" s="5" t="s">
+        <v>58</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added Filter for Customer in Add On Package
</commit_message>
<xml_diff>
--- a/ProductHistorical_TestData.xlsx
+++ b/ProductHistorical_TestData.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="4"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="LoginSignup" sheetId="1" state="visible" r:id="rId2"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="55">
   <si>
     <t xml:space="preserve">admin</t>
   </si>
@@ -32,7 +32,7 @@
     <t xml:space="preserve">WebData@123</t>
   </si>
   <si>
-    <t xml:space="preserve">Web Data 64</t>
+    <t xml:space="preserve">Web Data 49</t>
   </si>
   <si>
     <t xml:space="preserve">Marta</t>
@@ -59,7 +59,7 @@
     <t xml:space="preserve">United States Dollar</t>
   </si>
   <si>
-    <t xml:space="preserve">Child Web Data 64</t>
+    <t xml:space="preserve">Child Web Data 49</t>
   </si>
   <si>
     <t xml:space="preserve">H-50</t>
@@ -77,13 +77,13 @@
     <t xml:space="preserve">301520</t>
   </si>
   <si>
-    <t xml:space="preserve">Successfully created Child Web Data 64. You can now login with the username admin after your password is set. Password reset link is sent to your email.</t>
+    <t xml:space="preserve">Successfully created Child Web Data 49. You can now login with the username admin after your password is set. Password reset link is sent to your email.</t>
   </si>
   <si>
     <t xml:space="preserve">Currencies updated successfully.</t>
   </si>
   <si>
-    <t xml:space="preserve">Working as admin Child Web Data 64 X</t>
+    <t xml:space="preserve">Working as admin Child Web Data 49 X</t>
   </si>
   <si>
     <t xml:space="preserve">Test Category</t>
@@ -140,10 +140,37 @@
     <t xml:space="preserve">Total = C$93.00</t>
   </si>
   <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">Total = C$</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">123.00</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">Total = €96.00</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Total = €126.00</t>
+  </si>
+  <si>
     <t xml:space="preserve">'01/26/2017'</t>
   </si>
   <si>
-    <t xml:space="preserve">Working as admin Child Web Data 64 X</t>
+    <t xml:space="preserve">Working as admin Child Web Data 49 X</t>
   </si>
   <si>
     <t xml:space="preserve">Total = US$99.00</t>
@@ -155,6 +182,33 @@
     <t xml:space="preserve">Total = C$102.00</t>
   </si>
   <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">Total = C$</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">132.00</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">Total = €105.00</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Total = €135.00</t>
+  </si>
+  <si>
     <t xml:space="preserve">Total = US$108.00</t>
   </si>
   <si>
@@ -162,6 +216,33 @@
   </si>
   <si>
     <t xml:space="preserve">Total = C$111.00</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">Total = C$</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">141.00</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">Total = €114.00</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Total = €144.00</t>
   </si>
 </sst>
 </file>
@@ -370,15 +451,15 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="1:1"/>
+  <dimension ref="A1:AMJ1"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="N1" activeCellId="0" sqref="N1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="9.01481481481481"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="9.01"/>
   </cols>
   <sheetData>
     <row r="1" s="1" customFormat="true" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -455,7 +536,7 @@
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"Page &amp;P</oddFooter>
@@ -470,19 +551,19 @@
   </sheetPr>
   <dimension ref="A1:F1"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="G1" activeCellId="0" sqref="G1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="10.1925925925926"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="14.4037037037037"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="18.0296296296296"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="25.3814814814815"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="31.3592592592593"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="41.3518518518519"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="1" width="10.1925925925926"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="10.19"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="14.4"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="18.03"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="25.38"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="31.36"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="41.35"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="7" style="1" width="10.19"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -511,7 +592,7 @@
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -526,22 +607,22 @@
   </sheetPr>
   <dimension ref="A1:R9"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="O1" activeCellId="0" sqref="O1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="7.74074074074074"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="9.6037037037037"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="17.6407407407407"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="13.1296296296296"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="22.4407407407407"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="13.1296296296296"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="13.7185185185185"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="19.6962962962963"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="5.58518518518519"/>
-    <col collapsed="false" hidden="false" max="1025" min="10" style="1" width="9.6037037037037"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="7.74"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="9.6"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="17.64"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="13.13"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="22.44"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="13.13"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="13.72"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="19.7"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="5.59"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="10" style="1" width="9.6"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -812,7 +893,7 @@
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"Page &amp;P</oddFooter>
@@ -827,19 +908,19 @@
   </sheetPr>
   <dimension ref="A1:F3"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="E1" activeCellId="0" sqref="E1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="9.6037037037037"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="14.9925925925926"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="22.3444444444444"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="8.81851851851852"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="14.7"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="22.3444444444444"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="1" width="9.6037037037037"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="9.6"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="14.99"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="22.34"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="8.82"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="14.7"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="22.34"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="7" style="1" width="9.6"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -887,7 +968,7 @@
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"Page &amp;P</oddFooter>
@@ -902,24 +983,24 @@
   </sheetPr>
   <dimension ref="A1:M4"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I5" activeCellId="0" sqref="I5"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="E1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="I18" activeCellId="0" sqref="I18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="9.6037037037037"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="15.6777777777778"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="35.1814814814815"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="14.7"/>
-    <col collapsed="false" hidden="false" max="7" min="5" style="1" width="13.1296296296296"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="18.6111111111111"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="23.4740740740741"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="20.1666666666667"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="1" width="3.91851851851852"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="1" width="4.9962962962963"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="1" width="3.91851851851852"/>
-    <col collapsed="false" hidden="false" max="1025" min="14" style="1" width="9.6037037037037"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="9.6"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="15.68"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="35.18"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="14.7"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="5" style="1" width="13.13"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="18.61"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="23.47"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="20.17"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="1" width="12.47"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="1" width="14.67"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="1" width="14.12"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="14" style="1" width="9.6"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="20.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -953,17 +1034,17 @@
       <c r="J1" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="K1" s="5" t="n">
-        <v>123</v>
-      </c>
-      <c r="L1" s="5" t="n">
-        <v>96</v>
-      </c>
-      <c r="M1" s="5" t="n">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="2" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="K1" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="L1" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="M1" s="5" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C2" s="1" t="s">
         <v>11</v>
       </c>
@@ -971,7 +1052,7 @@
         <v>33</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="F2" s="1" t="s">
         <v>23</v>
@@ -979,7 +1060,7 @@
       <c r="G2" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="H2" s="6" t="s">
+      <c r="H2" s="5" t="s">
         <v>35</v>
       </c>
       <c r="I2" s="5" t="s">
@@ -988,19 +1069,19 @@
       <c r="J2" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="K2" s="5" t="n">
-        <v>123</v>
-      </c>
-      <c r="L2" s="5" t="n">
-        <v>96</v>
-      </c>
-      <c r="M2" s="5" t="n">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="K2" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="L2" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="M2" s="5" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C3" s="5" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="D3" s="5" t="s">
         <v>34</v>
@@ -1015,45 +1096,45 @@
         <v>27</v>
       </c>
       <c r="H3" s="5" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="I3" s="5" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="J3" s="5" t="s">
-        <v>42</v>
-      </c>
-      <c r="K3" s="5" t="n">
-        <v>132</v>
-      </c>
-      <c r="L3" s="5" t="n">
-        <v>105</v>
-      </c>
-      <c r="M3" s="5" t="n">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>45</v>
+      </c>
+      <c r="K3" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="L3" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="M3" s="5" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="21.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="E4" s="4" t="s">
         <v>30</v>
       </c>
       <c r="H4" s="5" t="s">
-        <v>43</v>
+        <v>49</v>
       </c>
       <c r="I4" s="5" t="s">
-        <v>44</v>
+        <v>50</v>
       </c>
       <c r="J4" s="5" t="s">
-        <v>45</v>
-      </c>
-      <c r="K4" s="5" t="n">
-        <v>141</v>
-      </c>
-      <c r="L4" s="5" t="n">
-        <v>114</v>
-      </c>
-      <c r="M4" s="5" t="n">
-        <v>144</v>
+        <v>51</v>
+      </c>
+      <c r="K4" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="L4" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="M4" s="5" t="s">
+        <v>54</v>
       </c>
     </row>
   </sheetData>
@@ -1062,7 +1143,7 @@
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"Page &amp;P</oddFooter>

</xml_diff>

<commit_message>
Changes in the Suite of Product Historical Test Plan
</commit_message>
<xml_diff>
--- a/ProductHistorical_TestData.xlsx
+++ b/ProductHistorical_TestData.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="4"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="LoginSignup" sheetId="1" state="visible" r:id="rId2"/>
@@ -15,234 +15,175 @@
     <sheet name="CreateOrder" sheetId="5" state="visible" r:id="rId6"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
-  <extLst>
-    <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
-      <loext:extCalcPr stringRefSyntax="CalcA1ExcelA1"/>
-    </ext>
-  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="55">
   <si>
-    <t xml:space="preserve">admin</t>
-  </si>
-  <si>
-    <t xml:space="preserve">WebData@123</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Web Data 49</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Marta</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Kauffman</t>
-  </si>
-  <si>
-    <t xml:space="preserve">345</t>
-  </si>
-  <si>
-    <t xml:space="preserve">354</t>
-  </si>
-  <si>
-    <t xml:space="preserve">3456</t>
-  </si>
-  <si>
-    <t xml:space="preserve">marta@weddatatech.in</t>
-  </si>
-  <si>
-    <t xml:space="preserve">English</t>
-  </si>
-  <si>
-    <t xml:space="preserve">United States Dollar</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Child Web Data 49</t>
-  </si>
-  <si>
-    <t xml:space="preserve">H-50</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DC,213</t>
-  </si>
-  <si>
-    <t xml:space="preserve">NewYork</t>
-  </si>
-  <si>
-    <t xml:space="preserve">United States</t>
-  </si>
-  <si>
-    <t xml:space="preserve">301520</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Successfully created Child Web Data 49. You can now login with the username admin after your password is set. Password reset link is sent to your email.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Currencies updated successfully.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Working as admin Child Web Data 49 X</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Test Category</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Test Product1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">'01/01/1970'</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Test Product2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Canadian Dollar</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Test Product3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Euro</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Test Product4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">'06/26/2018'</t>
-  </si>
-  <si>
-    <t xml:space="preserve">06/26/2018</t>
-  </si>
-  <si>
-    <t xml:space="preserve">'01/01/2020'</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Default</t>
-  </si>
-  <si>
-    <t xml:space="preserve">USD Customer</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CAD Customer</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Euro Customer</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Total = US$90.00</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Total = US$120.00</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Total = C$93.00</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">Total = C$</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">123.00</t>
-    </r>
-  </si>
-  <si>
-    <t xml:space="preserve">Total = €96.00</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Total = €126.00</t>
-  </si>
-  <si>
-    <t xml:space="preserve">'01/26/2017'</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Working as admin Child Web Data 49 X</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Total = US$99.00</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Total = US$129.00</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Total = C$102.00</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">Total = C$</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">132.00</t>
-    </r>
-  </si>
-  <si>
-    <t xml:space="preserve">Total = €105.00</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Total = €135.00</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Total = US$108.00</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Total = US$138.00</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Total = C$111.00</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">Total = C$</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">141.00</t>
-    </r>
-  </si>
-  <si>
-    <t xml:space="preserve">Total = €114.00</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Total = €144.00</t>
+    <t>admin</t>
+  </si>
+  <si>
+    <t>WebData@123</t>
+  </si>
+  <si>
+    <t>Web Data 1</t>
+  </si>
+  <si>
+    <t>Marta</t>
+  </si>
+  <si>
+    <t>Kauffman</t>
+  </si>
+  <si>
+    <t>345</t>
+  </si>
+  <si>
+    <t>354</t>
+  </si>
+  <si>
+    <t>3456</t>
+  </si>
+  <si>
+    <t>marta@weddatatech.in</t>
+  </si>
+  <si>
+    <t>English</t>
+  </si>
+  <si>
+    <t>United States Dollar</t>
+  </si>
+  <si>
+    <t>Child Web Data 1</t>
+  </si>
+  <si>
+    <t>H-50</t>
+  </si>
+  <si>
+    <t>DC,213</t>
+  </si>
+  <si>
+    <t>NewYork</t>
+  </si>
+  <si>
+    <t>United States</t>
+  </si>
+  <si>
+    <t>301520</t>
+  </si>
+  <si>
+    <t>Successfully created Child Web Data 1. You can now login with the username admin after your password is set. Password reset link is sent to your email.</t>
+  </si>
+  <si>
+    <t>Currencies updated successfully.</t>
+  </si>
+  <si>
+    <t>Working as admin Child Web Data 1 X</t>
+  </si>
+  <si>
+    <t>Historical Category</t>
+  </si>
+  <si>
+    <t>Historical Product1</t>
+  </si>
+  <si>
+    <t>'01/01/1970'</t>
+  </si>
+  <si>
+    <t>Historical Product2</t>
+  </si>
+  <si>
+    <t>Canadian Dollar</t>
+  </si>
+  <si>
+    <t>Historical Product3</t>
+  </si>
+  <si>
+    <t>Euro</t>
+  </si>
+  <si>
+    <t>Historical Product4</t>
+  </si>
+  <si>
+    <t>'06/26/2018'</t>
+  </si>
+  <si>
+    <t>06/26/2018</t>
+  </si>
+  <si>
+    <t>'01/01/2020'</t>
+  </si>
+  <si>
+    <t>Default</t>
+  </si>
+  <si>
+    <t>USD Customer</t>
+  </si>
+  <si>
+    <t>CAD Customer</t>
+  </si>
+  <si>
+    <t>Euro Customer</t>
+  </si>
+  <si>
+    <t>Total = US$90.00</t>
+  </si>
+  <si>
+    <t>Total = US$120.00</t>
+  </si>
+  <si>
+    <t>Total = C$93.00</t>
+  </si>
+  <si>
+    <t>Total = C$123.00</t>
+  </si>
+  <si>
+    <t>Total = €96.00</t>
+  </si>
+  <si>
+    <t>Total = €126.00</t>
+  </si>
+  <si>
+    <t>'01/26/2017'</t>
+  </si>
+  <si>
+    <t>Working as admin Child Web Data 1 X</t>
+  </si>
+  <si>
+    <t>Total = US$99.00</t>
+  </si>
+  <si>
+    <t>Total = US$129.00</t>
+  </si>
+  <si>
+    <t>Total = C$102.00</t>
+  </si>
+  <si>
+    <t>Total = C$132.00</t>
+  </si>
+  <si>
+    <t>Total = €105.00</t>
+  </si>
+  <si>
+    <t>Total = €135.00</t>
+  </si>
+  <si>
+    <t>Total = US$108.00</t>
+  </si>
+  <si>
+    <t>Total = US$138.00</t>
+  </si>
+  <si>
+    <t>Total = C$111.00</t>
+  </si>
+  <si>
+    <t>Total = C$141.00</t>
+  </si>
+  <si>
+    <t>Total = €114.00</t>
+  </si>
+  <si>
+    <t>Total = €144.00</t>
   </si>
 </sst>
 </file>
@@ -250,10 +191,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="2">
-    <numFmt numFmtId="164" formatCode="General"/>
+    <numFmt numFmtId="164" formatCode="GENERAL"/>
     <numFmt numFmtId="165" formatCode="DD/MM/YY"/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="6">
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
@@ -291,12 +232,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -344,7 +279,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="6">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -366,10 +301,6 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -451,15 +382,15 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:AMJ1"/>
+  <dimension ref="1:1"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="N1" activeCellId="0" sqref="N1"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="N1" activeCellId="1" sqref="C1:D1 N1 U1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="9.01"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="9.00740740740741"/>
   </cols>
   <sheetData>
     <row r="1" s="1" customFormat="true" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -536,7 +467,7 @@
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"Page &amp;P</oddFooter>
@@ -551,19 +482,19 @@
   </sheetPr>
   <dimension ref="A1:F1"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G1" activeCellId="0" sqref="G1"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G1" activeCellId="3" sqref="C1:D1 N1 U1 G1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="10.19"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="14.4"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="18.03"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="25.38"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="31.36"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="41.35"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="7" style="1" width="10.19"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="10.1925925925926"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="14.4"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="18.0296296296296"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="25.3814814814815"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="31.3592592592593"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="41.3518518518519"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="1" width="10.1925925925926"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -592,7 +523,7 @@
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -607,22 +538,22 @@
   </sheetPr>
   <dimension ref="A1:R9"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="O1" activeCellId="0" sqref="O1"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D1" activeCellId="0" sqref="C1:D1 N1 U1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="7.74"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="9.6"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="17.64"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="13.13"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="22.44"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="13.13"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="13.72"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="19.7"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="5.59"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="10" style="1" width="9.6"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="7.74074074074074"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="9.5962962962963"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="17.6407407407407"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="13.1296296296296"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="22.4407407407407"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="13.1296296296296"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="13.7185185185185"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="19.6962962962963"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="5.58518518518519"/>
+    <col collapsed="false" hidden="false" max="1025" min="10" style="1" width="9.5962962962963"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -893,7 +824,7 @@
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"Page &amp;P</oddFooter>
@@ -908,19 +839,19 @@
   </sheetPr>
   <dimension ref="A1:F3"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E1" activeCellId="0" sqref="E1"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E1" activeCellId="3" sqref="C1:D1 N1 U1 E1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="9.6"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="14.99"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="22.34"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="8.82"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="14.7"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="22.34"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="7" style="1" width="9.6"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="9.5962962962963"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="14.9851851851852"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="22.3444444444444"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="8.81851851851852"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="14.7"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="22.3444444444444"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="1" width="9.5962962962963"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -968,7 +899,7 @@
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"Page &amp;P</oddFooter>
@@ -983,24 +914,24 @@
   </sheetPr>
   <dimension ref="A1:M4"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="E1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I18" activeCellId="0" sqref="I18"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F1" activeCellId="3" sqref="C1:D1 N1 U1 F1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="9.6"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="15.68"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="35.18"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="14.7"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="5" style="1" width="13.13"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="18.61"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="23.47"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="20.17"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="1" width="12.47"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="1" width="14.67"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="1" width="14.12"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="14" style="1" width="9.6"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="9.5962962962963"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="15.6777777777778"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="35.1814814814815"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="14.7"/>
+    <col collapsed="false" hidden="false" max="7" min="5" style="1" width="13.1296296296296"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="18.6111111111111"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="23.4740740740741"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="20.1666666666667"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="1" width="12.4703703703704"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="1" width="14.6740740740741"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="1" width="14.1185185185185"/>
+    <col collapsed="false" hidden="false" max="1025" min="14" style="1" width="9.5962962962963"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="20.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1034,7 +965,7 @@
       <c r="J1" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="K1" s="6" t="s">
+      <c r="K1" s="5" t="s">
         <v>38</v>
       </c>
       <c r="L1" s="5" t="s">
@@ -1069,7 +1000,7 @@
       <c r="J2" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="K2" s="6" t="s">
+      <c r="K2" s="5" t="s">
         <v>38</v>
       </c>
       <c r="L2" s="5" t="s">
@@ -1104,7 +1035,7 @@
       <c r="J3" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="K3" s="6" t="s">
+      <c r="K3" s="5" t="s">
         <v>46</v>
       </c>
       <c r="L3" s="5" t="s">
@@ -1127,7 +1058,7 @@
       <c r="J4" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="K4" s="6" t="s">
+      <c r="K4" s="5" t="s">
         <v>52</v>
       </c>
       <c r="L4" s="5" t="s">
@@ -1143,7 +1074,7 @@
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"Page &amp;P</oddFooter>

</xml_diff>

<commit_message>
Remove the Redundancy from the Product Historical Scenario
</commit_message>
<xml_diff>
--- a/ProductHistorical_TestData.xlsx
+++ b/ProductHistorical_TestData.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="LoginSignup" sheetId="1" state="visible" r:id="rId2"/>
@@ -15,175 +15,177 @@
     <sheet name="CreateOrder" sheetId="5" state="visible" r:id="rId6"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
+  <extLst>
+    <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
+      <loext:extCalcPr stringRefSyntax="CalcA1ExcelA1"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="55">
-  <si>
-    <t>admin</t>
-  </si>
-  <si>
-    <t>WebData@123</t>
-  </si>
-  <si>
-    <t>Web Data 1</t>
-  </si>
-  <si>
-    <t>Marta</t>
-  </si>
-  <si>
-    <t>Kauffman</t>
-  </si>
-  <si>
-    <t>345</t>
-  </si>
-  <si>
-    <t>354</t>
-  </si>
-  <si>
-    <t>3456</t>
-  </si>
-  <si>
-    <t>marta@weddatatech.in</t>
-  </si>
-  <si>
-    <t>English</t>
-  </si>
-  <si>
-    <t>United States Dollar</t>
-  </si>
-  <si>
-    <t>Child Web Data 1</t>
-  </si>
-  <si>
-    <t>H-50</t>
-  </si>
-  <si>
-    <t>DC,213</t>
-  </si>
-  <si>
-    <t>NewYork</t>
-  </si>
-  <si>
-    <t>United States</t>
-  </si>
-  <si>
-    <t>301520</t>
-  </si>
-  <si>
-    <t>Successfully created Child Web Data 1. You can now login with the username admin after your password is set. Password reset link is sent to your email.</t>
-  </si>
-  <si>
-    <t>Currencies updated successfully.</t>
-  </si>
-  <si>
-    <t>Working as admin Child Web Data 1 X</t>
-  </si>
-  <si>
-    <t>Historical Category</t>
-  </si>
-  <si>
-    <t>Historical Product1</t>
-  </si>
-  <si>
-    <t>'01/01/1970'</t>
-  </si>
-  <si>
-    <t>Historical Product2</t>
-  </si>
-  <si>
-    <t>Canadian Dollar</t>
-  </si>
-  <si>
-    <t>Historical Product3</t>
-  </si>
-  <si>
-    <t>Euro</t>
-  </si>
-  <si>
-    <t>Historical Product4</t>
-  </si>
-  <si>
-    <t>'06/26/2018'</t>
-  </si>
-  <si>
-    <t>06/26/2018</t>
-  </si>
-  <si>
-    <t>'01/01/2020'</t>
-  </si>
-  <si>
-    <t>Default</t>
-  </si>
-  <si>
-    <t>USD Customer</t>
-  </si>
-  <si>
-    <t>CAD Customer</t>
-  </si>
-  <si>
-    <t>Euro Customer</t>
-  </si>
-  <si>
-    <t>Total = US$90.00</t>
-  </si>
-  <si>
-    <t>Total = US$120.00</t>
-  </si>
-  <si>
-    <t>Total = C$93.00</t>
-  </si>
-  <si>
-    <t>Total = C$123.00</t>
-  </si>
-  <si>
-    <t>Total = €96.00</t>
-  </si>
-  <si>
-    <t>Total = €126.00</t>
-  </si>
-  <si>
-    <t>'01/26/2017'</t>
-  </si>
-  <si>
-    <t>Working as admin Child Web Data 1 X</t>
-  </si>
-  <si>
-    <t>Total = US$99.00</t>
-  </si>
-  <si>
-    <t>Total = US$129.00</t>
-  </si>
-  <si>
-    <t>Total = C$102.00</t>
-  </si>
-  <si>
-    <t>Total = C$132.00</t>
-  </si>
-  <si>
-    <t>Total = €105.00</t>
-  </si>
-  <si>
-    <t>Total = €135.00</t>
-  </si>
-  <si>
-    <t>Total = US$108.00</t>
-  </si>
-  <si>
-    <t>Total = US$138.00</t>
-  </si>
-  <si>
-    <t>Total = C$111.00</t>
-  </si>
-  <si>
-    <t>Total = C$141.00</t>
-  </si>
-  <si>
-    <t>Total = €114.00</t>
-  </si>
-  <si>
-    <t>Total = €144.00</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="54">
+  <si>
+    <t xml:space="preserve">admin</t>
+  </si>
+  <si>
+    <t xml:space="preserve">WebData@123</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Web Data 5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Marta</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kauffman</t>
+  </si>
+  <si>
+    <t xml:space="preserve">345</t>
+  </si>
+  <si>
+    <t xml:space="preserve">354</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3456</t>
+  </si>
+  <si>
+    <t xml:space="preserve">marta@weddatatech.in</t>
+  </si>
+  <si>
+    <t xml:space="preserve">English</t>
+  </si>
+  <si>
+    <t xml:space="preserve">United States Dollar</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Child Web Data 5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">H-50</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DC,213</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NewYork</t>
+  </si>
+  <si>
+    <t xml:space="preserve">United States</t>
+  </si>
+  <si>
+    <t xml:space="preserve">301520</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Successfully created Child Web Data 5. You can now login with the username admin after your password is set. Password reset link is sent to your email.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Currencies updated successfully.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Working as admin Child Web Data 5 X</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Historical Category</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Historical Product1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">'01/01/1970'</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Historical Product2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Canadian Dollar</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Historical Product3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Euro</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Historical Product4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">'01/01/2019'</t>
+  </si>
+  <si>
+    <t xml:space="preserve">'01/01/2025'</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Default</t>
+  </si>
+  <si>
+    <t xml:space="preserve">USD Customer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CAD Customer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Euro Customer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Total = US$90.00</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Total = US$120.00</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Total = C$93.00</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Total = C$123.00</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Total = €96.00</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Total = €126.00</t>
+  </si>
+  <si>
+    <t xml:space="preserve">'01/26/2018'</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Working as admin Child Web Data 5 X</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Total = US$99.00</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Total = US$129.00</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Total = C$102.00</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Total = C$132.00</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Total = €105.00</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Total = €135.00</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Total = US$108.00</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Total = US$138.00</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Total = C$111.00</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Total = C$141.00</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Total = €114.00</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Total = €144.00</t>
   </si>
 </sst>
 </file>
@@ -191,7 +193,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="2">
-    <numFmt numFmtId="164" formatCode="GENERAL"/>
+    <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="DD/MM/YY"/>
   </numFmts>
   <fonts count="6">
@@ -382,15 +384,15 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="1:1"/>
+  <dimension ref="A1:AMJ1"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="N1" activeCellId="1" sqref="C1:D1 N1 U1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="N1" activeCellId="0" sqref="N1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="9.00740740740741"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="9.01"/>
   </cols>
   <sheetData>
     <row r="1" s="1" customFormat="true" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -467,7 +469,7 @@
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"Page &amp;P</oddFooter>
@@ -482,19 +484,19 @@
   </sheetPr>
   <dimension ref="A1:F1"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G1" activeCellId="3" sqref="C1:D1 N1 U1 G1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C1" activeCellId="0" sqref="C1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="10.1925925925926"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="14.4"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="18.0296296296296"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="25.3814814814815"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="31.3592592592593"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="41.3518518518519"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="1" width="10.1925925925926"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="10.19"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="14.4"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="18.03"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="25.38"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="31.36"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="41.35"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="7" style="1" width="10.19"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -523,7 +525,7 @@
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -538,22 +540,22 @@
   </sheetPr>
   <dimension ref="A1:R9"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D1" activeCellId="0" sqref="C1:D1 N1 U1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G7" activeCellId="0" sqref="G7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="7.74074074074074"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="9.5962962962963"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="17.6407407407407"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="13.1296296296296"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="22.4407407407407"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="13.1296296296296"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="13.7185185185185"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="19.6962962962963"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="5.58518518518519"/>
-    <col collapsed="false" hidden="false" max="1025" min="10" style="1" width="9.5962962962963"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="7.74"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="9.6"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="17.64"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="13.13"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="22.44"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="13.13"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="13.72"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="19.7"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="5.59"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="10" style="1" width="9.6"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -690,7 +692,7 @@
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="G5" s="4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="H5" s="1" t="s">
         <v>24</v>
@@ -716,7 +718,7 @@
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="G6" s="4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="H6" s="1" t="s">
         <v>26</v>
@@ -742,7 +744,7 @@
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="G7" s="4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="H7" s="4" t="s">
         <v>10</v>
@@ -768,7 +770,7 @@
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="G8" s="4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="H8" s="1" t="s">
         <v>24</v>
@@ -794,7 +796,7 @@
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="G9" s="4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="H9" s="1" t="s">
         <v>26</v>
@@ -824,7 +826,7 @@
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"Page &amp;P</oddFooter>
@@ -839,19 +841,19 @@
   </sheetPr>
   <dimension ref="A1:F3"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E1" activeCellId="3" sqref="C1:D1 N1 U1 E1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E1" activeCellId="0" sqref="E1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="9.5962962962963"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="14.9851851851852"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="22.3444444444444"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="8.81851851851852"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="14.7"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="22.3444444444444"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="1" width="9.5962962962963"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="9.6"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="14.99"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="22.34"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="8.82"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="14.7"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="22.34"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="7" style="1" width="9.6"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -865,10 +867,10 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>31</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>32</v>
       </c>
       <c r="F1" s="5" t="s">
         <v>10</v>
@@ -879,7 +881,7 @@
         <v>11</v>
       </c>
       <c r="E2" s="5" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="F2" s="5" t="s">
         <v>24</v>
@@ -887,7 +889,7 @@
     </row>
     <row r="3" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E3" s="5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F3" s="5" t="s">
         <v>26</v>
@@ -899,7 +901,7 @@
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"Page &amp;P</oddFooter>
@@ -914,24 +916,25 @@
   </sheetPr>
   <dimension ref="A1:M4"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F1" activeCellId="3" sqref="C1:D1 N1 U1 F1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D8" activeCellId="0" sqref="D8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="9.5962962962963"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="15.6777777777778"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="35.1814814814815"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="14.7"/>
-    <col collapsed="false" hidden="false" max="7" min="5" style="1" width="13.1296296296296"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="18.6111111111111"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="23.4740740740741"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="20.1666666666667"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="1" width="12.4703703703704"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="1" width="14.6740740740741"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="1" width="14.1185185185185"/>
-    <col collapsed="false" hidden="false" max="1025" min="14" style="1" width="9.5962962962963"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="9.6"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="15.68"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="35.18"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="14.7"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="13.13"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="6" style="1" width="18.34"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="18.61"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="23.47"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="20.17"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="1" width="12.47"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="1" width="14.67"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="1" width="14.12"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="14" style="1" width="9.6"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="20.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -945,127 +948,124 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E1" s="4" t="s">
         <v>22</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="G1" s="1" t="s">
         <v>21</v>
       </c>
       <c r="H1" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="I1" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="I1" s="5" t="s">
+      <c r="J1" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="J1" s="5" t="s">
+      <c r="K1" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="K1" s="5" t="s">
+      <c r="L1" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="L1" s="5" t="s">
+      <c r="M1" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="M1" s="5" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="2" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="2" customFormat="false" ht="29.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C2" s="1" t="s">
         <v>11</v>
       </c>
       <c r="D2" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="H2" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="I2" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="J2" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="K2" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="L2" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="M2" s="5" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="29.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C3" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="D3" s="5" t="s">
         <v>33</v>
-      </c>
-      <c r="E2" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="H2" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="I2" s="5" t="s">
-        <v>36</v>
-      </c>
-      <c r="J2" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="K2" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="L2" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="M2" s="5" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C3" s="5" t="s">
-        <v>42</v>
-      </c>
-      <c r="D3" s="5" t="s">
-        <v>34</v>
       </c>
       <c r="E3" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="F3" s="1" t="s">
-        <v>27</v>
-      </c>
       <c r="G3" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="H3" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="I3" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="I3" s="5" t="s">
+      <c r="J3" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="J3" s="5" t="s">
+      <c r="K3" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="K3" s="5" t="s">
+      <c r="L3" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="L3" s="5" t="s">
+      <c r="M3" s="5" t="s">
         <v>47</v>
-      </c>
-      <c r="M3" s="5" t="s">
-        <v>48</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="21.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="E4" s="4" t="s">
-        <v>30</v>
+        <v>29</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>27</v>
       </c>
       <c r="H4" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="I4" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="I4" s="5" t="s">
+      <c r="J4" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="J4" s="5" t="s">
+      <c r="K4" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="K4" s="5" t="s">
+      <c r="L4" s="5" t="s">
         <v>52</v>
       </c>
-      <c r="L4" s="5" t="s">
+      <c r="M4" s="5" t="s">
         <v>53</v>
-      </c>
-      <c r="M4" s="5" t="s">
-        <v>54</v>
       </c>
     </row>
   </sheetData>
@@ -1074,7 +1074,7 @@
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"Page &amp;P</oddFooter>

</xml_diff>